<commit_message>
add data - set sample sizes and if is in standard rotation
</commit_message>
<xml_diff>
--- a/CROSS_SECTION_ANALYSIS/booster_pack_prices_12.4.25.xlsx
+++ b/CROSS_SECTION_ANALYSIS/booster_pack_prices_12.4.25.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janhr\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janhr\Repos\Pokemon_Market_Efficiency_Final\CROSS_SECTION_ANALYSIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7459C66E-FC86-4325-8EDC-A12D5BA8A92A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152A30BD-671B-402A-9045-03F167BA8C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>Booster Pack</t>
   </si>
@@ -125,13 +125,28 @@
   </si>
   <si>
     <t>Stellar Crown Booster Pack</t>
+  </si>
+  <si>
+    <t>Booster Sample No</t>
+  </si>
+  <si>
+    <t>8000+</t>
+  </si>
+  <si>
+    <t>1900+</t>
+  </si>
+  <si>
+    <t>1500+</t>
+  </si>
+  <si>
+    <t>Is Standard Rotation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,6 +160,15 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -183,11 +207,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,287 +518,494 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>12.13</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" s="3">
+        <v>7020</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>13.65</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" s="3">
+        <v>2088</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <v>14.47</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" s="3">
+        <v>2010</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <v>45.48</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5" s="3">
+        <v>1536</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <v>9.69</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6" s="3">
+        <v>1530</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
         <v>24.79</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7" s="3">
+        <v>1674</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
         <v>20.85</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8" s="3">
+        <v>1264</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
         <v>27.51</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9" s="3">
+        <v>1480</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10">
         <v>23.68</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10" s="3">
+        <v>1274</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11">
         <v>105.71</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C11" s="3">
+        <v>872</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12">
         <v>35.119999999999997</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C12" s="3">
+        <v>3888</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13">
         <v>31.26</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C13" s="3">
+        <v>3672</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14">
         <v>27.44</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C14" s="3">
+        <v>1580</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15">
         <v>31.62</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C15" s="3">
+        <v>3136</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16">
         <v>6.48</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16" s="3">
+        <v>4628</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17">
         <v>5.78</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17" s="3">
+        <v>2736</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18">
         <v>6.45</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18" s="3">
+        <v>5040</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19">
         <v>12.3</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19" s="3">
+        <v>3192</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20">
         <v>9.4600000000000009</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20" s="3">
+        <v>2187</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21">
         <v>21.47</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22">
         <v>5.9</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23">
         <v>8.82</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24">
         <v>6.51</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25">
         <v>8.89</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26">
         <v>5.49</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27">
         <v>6.56</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28">
         <v>5.91</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29">
         <v>10.66</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30">
         <v>5.7</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31">
         <v>9.19</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32">
         <v>5.47</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33">
         <v>6.57</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34">
         <v>5.73</v>
+      </c>
+      <c r="C34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>